<commit_message>
Some changes and fix issue
- Changes configuration
- Fix warning message when add the data (timezone)
- Fix empty cells must not be inserted while import excel (Pegawai, Posisi, and
Kota)
</commit_message>
<xml_diff>
--- a/assets/excel/Data Pegawai.xlsx
+++ b/assets/excel/Data Pegawai.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -38,10 +38,10 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Samsul Huda</t>
-  </si>
-  <si>
-    <t>085234640114</t>
+    <t>Hariyanto</t>
+  </si>
+  <si>
+    <t>081233072122</t>
   </si>
   <si>
     <t>Antony Febriansyah Hartono</t>
@@ -62,10 +62,10 @@
     <t>085736333728</t>
   </si>
   <si>
-    <t>Tolkha Hasan</t>
-  </si>
-  <si>
-    <t>081233072122</t>
+    <t>Reanaldo Revanzah Putra</t>
+  </si>
+  <si>
+    <t>085745966707</t>
   </si>
   <si>
     <t>Mustofa Halim</t>
@@ -86,18 +86,6 @@
     <t>085749535400</t>
   </si>
   <si>
-    <t>Wawan Dwi Prasetyo</t>
-  </si>
-  <si>
-    <t>085745966707</t>
-  </si>
-  <si>
-    <t>Achmad Chadil Auwfar</t>
-  </si>
-  <si>
-    <t>08984119934</t>
-  </si>
-  <si>
     <t>Rizal Ferdian</t>
   </si>
   <si>
@@ -108,6 +96,15 @@
   </si>
   <si>
     <t>083834657395</t>
+  </si>
+  <si>
+    <t>966a502429edc5a4e9222942eec72c57</t>
+  </si>
+  <si>
+    <t>Amirah Rahmani</t>
+  </si>
+  <si>
+    <t>087654321234</t>
   </si>
 </sst>
 </file>
@@ -446,7 +443,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -580,7 +577,7 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -663,7 +660,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -672,13 +669,13 @@
         <v>24</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -686,7 +683,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -701,55 +698,32 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12">
-        <v>8</v>
+      <c r="A12" t="s">
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13">
         <v>1</v>
       </c>
     </row>

</xml_diff>